<commit_message>
Dataframe con carrefour ok
</commit_message>
<xml_diff>
--- a/codigos.xlsx
+++ b/codigos.xlsx
@@ -16,6 +16,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>ESPADOL DETTOL ALOE VERA 80 GR JAB</t>
+  </si>
+  <si>
+    <t>ISSUE TRATAMIENTO CAPILAR BRILLO EXTREMO X 150</t>
+  </si>
+  <si>
+    <t>COLGATE HERBAL C/MINERALES 90GR DEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UREADIN MANOS CREAM PLUS CRE 50 ML </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -352,24 +369,36 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>7798339190105</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7793008017387</v>
       </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7509546692197</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8429420152120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>